<commit_message>
fix upload logic, upload samples and material table localization
</commit_message>
<xml_diff>
--- a/public/upload-sample.xlsx
+++ b/public/upload-sample.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,44 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\masterplanner\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DABF620-431E-4528-A145-030F012DDBA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{940BA42B-E11A-4E4C-8D1D-3624DA44F713}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="sample" sheetId="1" r:id="rId1"/>
+    <sheet name="upload-sample" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
   <si>
+    <t>Type</t>
+  </si>
+  <si>
     <t>Birth year</t>
   </si>
   <si>
-    <t>Club</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
     <t>Hotel</t>
   </si>
   <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Tournaments</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Arrival date</t>
   </si>
   <si>
@@ -55,28 +46,40 @@
     <t>Ocnarescu Victor</t>
   </si>
   <si>
-    <t>Clubul Central de Sah Bucuresti</t>
-  </si>
-  <si>
-    <t>Hotel Arad</t>
-  </si>
-  <si>
-    <t>Arad Open;Arad U1900</t>
-  </si>
-  <si>
-    <t>Informatii de test</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>player</t>
+  </si>
+  <si>
+    <t>Georgescu Tiberiu-Marian</t>
+  </si>
+  <si>
+    <t>Posedaru Bogdan</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t>FM</t>
+  </si>
+  <si>
+    <t>Chess Coders Cup</t>
+  </si>
+  <si>
+    <t>Room type</t>
+  </si>
+  <si>
+    <t>Main tournament</t>
+  </si>
+  <si>
+    <t>Federation</t>
+  </si>
+  <si>
+    <t>ROU</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -911,84 +914,127 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2">
-        <v>1989</v>
+      <c r="C2" t="s">
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>1991</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
-        <v>14</v>
+      <c r="I2" s="1">
+        <v>44098</v>
       </c>
       <c r="J2" s="1">
-        <v>43732</v>
-      </c>
-      <c r="K2" s="1">
-        <v>43733</v>
+        <v>44099</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>1989</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1">
+        <v>44098</v>
+      </c>
+      <c r="J3" s="1">
+        <v>44099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4">
+        <v>1990</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="1">
+        <v>44099</v>
+      </c>
+      <c r="J4" s="1">
+        <v>44100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>